<commit_message>
Merge overwrote wrong version
</commit_message>
<xml_diff>
--- a/data/Budge.xlsx
+++ b/data/Budge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abowers\Documents\GitHub\writings\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abowers\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -373,8 +373,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -418,12 +424,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,7 +714,7 @@
   <dimension ref="B1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I5" sqref="I5:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,105 +732,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D1" s="23">
+      <c r="D1" s="5">
         <v>2016</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="24" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="23">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="5">
         <v>2017</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="I2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="20">
+      <c r="B3" s="22">
         <v>12</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="7">
         <v>2036.83</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="7">
         <v>24441.96</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="13">
         <f>E3/E$26</f>
         <v>0.28957318037576335</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>-170</v>
       </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H22" si="0">K3-E3</f>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H23" si="0">K3-E3</f>
         <v>-2040</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="9">
         <f>(1-(J3/D3))*-1</f>
         <v>-8.3463028333243372E-2</v>
       </c>
-      <c r="J3" s="4">
-        <f t="shared" ref="J3:J22" si="1">D3+G3</f>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J24" si="1">D3+G3</f>
         <v>1866.83</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="6">
         <f>J3*12</f>
         <v>22401.96</v>
       </c>
-      <c r="L3" s="11">
-        <f t="shared" ref="L3:L23" si="2">K3/K$26</f>
+      <c r="L3" s="13">
+        <f t="shared" ref="L3:L24" si="2">K3/K$26</f>
         <v>0.29566924685905305</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M22" si="3">C3</f>
+        <f t="shared" ref="M3:M23" si="3">C3</f>
         <v>Mortgage &amp; Rent</v>
       </c>
       <c r="N3" t="s">
@@ -838,42 +838,42 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="22">
         <v>287</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="7">
         <v>858.36083333333329</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="7">
         <v>10300.33</v>
       </c>
-      <c r="F4" s="11">
-        <f t="shared" ref="F4:F23" si="4">E4/E$26</f>
+      <c r="F4" s="13">
+        <f t="shared" ref="F4:F24" si="4">E4/E$26</f>
         <v>0.12203192039508642</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>-85</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <f t="shared" si="0"/>
         <v>-1020</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="9">
         <f>(1-(J4/D4))*-1</f>
         <v>-9.9025953537410949E-2</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="6">
         <f t="shared" si="1"/>
         <v>773.36083333333329</v>
       </c>
-      <c r="K4" s="4">
-        <f t="shared" ref="K4:K23" si="5">J4*12</f>
+      <c r="K4" s="6">
+        <f t="shared" ref="K4:K24" si="5">J4*12</f>
         <v>9280.33</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="13">
         <f t="shared" si="2"/>
         <v>0.12248518351534758</v>
       </c>
@@ -883,42 +883,42 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="22">
         <v>414</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="7">
         <v>674.47416666666663</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="7">
         <v>8093.69</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <f t="shared" si="4"/>
         <v>9.5889018486058894E-2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>-175</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>-2100</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="9">
         <f t="shared" ref="I5:I22" si="6">(1-(J5/D5))*-1</f>
         <v>-0.25946138287974951</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="6">
         <f t="shared" si="1"/>
         <v>499.47416666666663</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="6">
         <f t="shared" si="5"/>
         <v>5993.69</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="13">
         <f t="shared" si="2"/>
         <v>7.9106908868984568E-2</v>
       </c>
@@ -931,42 +931,42 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="22">
         <v>71</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="7">
         <v>451.24416666666667</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="7">
         <v>5414.93</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="13">
         <f t="shared" si="4"/>
         <v>6.4152731679952529E-2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>-50</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
         <v>-600</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="9">
         <f t="shared" si="6"/>
         <v>-0.11080475647884647</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="6">
         <f t="shared" si="1"/>
         <v>401.24416666666667</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="6">
         <f t="shared" si="5"/>
         <v>4814.93</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="13">
         <f t="shared" si="2"/>
         <v>6.3549204032998019E-2</v>
       </c>
@@ -979,42 +979,42 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+      <c r="B7" s="22">
         <v>123</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="7">
         <v>342.31916666666666</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="7">
         <v>4107.83</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="13">
         <f t="shared" si="4"/>
         <v>4.8667021693144574E-2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>-100</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>-1200</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="9">
         <f t="shared" si="6"/>
         <v>-0.29212503925430211</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
         <v>242.31916666666666</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="6">
         <f t="shared" si="5"/>
         <v>2907.83</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="13">
         <f t="shared" si="2"/>
         <v>3.8378601965817286E-2</v>
       </c>
@@ -1027,42 +1027,42 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
+      <c r="B8" s="22">
         <v>36</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="7">
         <v>284.78666666666669</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="7">
         <v>3417.44</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="13">
         <f t="shared" si="4"/>
         <v>4.0487709232129861E-2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>-30</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>-359.99999999999955</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="9">
         <f t="shared" si="6"/>
         <v>-0.10534201039374502</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="6">
         <f t="shared" si="1"/>
         <v>254.78666666666669</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="6">
         <f t="shared" si="5"/>
         <v>3057.4400000000005</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="13">
         <f t="shared" si="2"/>
         <v>4.0353209367249267E-2</v>
       </c>
@@ -1075,42 +1075,42 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="20">
+      <c r="B9" s="22">
         <v>88</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="7">
         <v>281.77833333333336</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="7">
         <v>3381.34</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="13">
         <f t="shared" si="4"/>
         <v>4.0060018825486328E-2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>-75</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <f t="shared" si="0"/>
         <v>-900</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="9">
         <f t="shared" si="6"/>
         <v>-0.2661666676524691</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="6">
         <f t="shared" si="1"/>
         <v>206.77833333333336</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="6">
         <f t="shared" si="5"/>
         <v>2481.34</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="13">
         <f t="shared" si="2"/>
         <v>3.2749631237679322E-2</v>
       </c>
@@ -1123,42 +1123,42 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="20">
+      <c r="B10" s="22">
         <v>48</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="7">
         <v>273.33999999999997</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="7">
         <v>3280.08</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="13">
         <f t="shared" si="4"/>
         <v>3.8860353158541049E-2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <v>-10</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <f t="shared" si="0"/>
         <v>-120</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="9">
         <f t="shared" si="6"/>
         <v>-3.6584473549425622E-2</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="6">
         <f t="shared" si="1"/>
         <v>263.33999999999997</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="6">
         <f t="shared" si="5"/>
         <v>3160.08</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="13">
         <f t="shared" si="2"/>
         <v>4.1707889560304384E-2</v>
       </c>
@@ -1171,42 +1171,42 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
+      <c r="B11" s="22">
         <v>74</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="7">
         <v>257.74083333333334</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="7">
         <v>3092.89</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="13">
         <f t="shared" si="4"/>
         <v>3.6642642155227924E-2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>-25</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
         <v>-299.99999999999955</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="9">
         <f t="shared" si="6"/>
         <v>-9.6996660081671182E-2</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="6">
         <f t="shared" si="1"/>
         <v>232.74083333333334</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="6">
         <f t="shared" si="5"/>
         <v>2792.8900000000003</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="13">
         <f t="shared" si="2"/>
         <v>3.6861581882129096E-2</v>
       </c>
@@ -1219,42 +1219,42 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+      <c r="B12" s="22">
         <v>4</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="7">
         <v>255.98916666666665</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="7">
         <v>3071.87</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="13">
         <f t="shared" si="4"/>
         <v>3.6393610234240467E-2</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <v>-115</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>-1380</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="9">
         <f t="shared" si="6"/>
         <v>-0.44923776071253019</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="6">
         <f t="shared" si="1"/>
         <v>140.98916666666665</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="6">
         <f t="shared" si="5"/>
         <v>1691.87</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="13">
         <f t="shared" si="2"/>
         <v>2.2329917948403891E-2</v>
       </c>
@@ -1267,37 +1267,40 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
+      <c r="B13" s="22">
         <v>24</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="7">
         <v>220.88333333333333</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="7">
         <v>2650.6</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="13">
         <f t="shared" si="4"/>
         <v>3.1402664594165047E-2</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="7">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="6">
         <f t="shared" si="1"/>
         <v>220.88333333333333</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="6">
         <f t="shared" si="5"/>
         <v>2650.6</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="13">
         <f t="shared" si="2"/>
         <v>3.4983586513171433E-2</v>
       </c>
@@ -1310,37 +1313,40 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="20">
+      <c r="B14" s="22">
         <v>12</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="7">
         <v>218.17</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="7">
         <v>2618.04</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="13">
         <f t="shared" si="4"/>
         <v>3.1016913911607887E-2</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="7">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="6">
         <f t="shared" si="1"/>
         <v>218.17</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="6">
         <f t="shared" si="5"/>
         <v>2618.04</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="13">
         <f t="shared" si="2"/>
         <v>3.4553847745772033E-2</v>
       </c>
@@ -1350,42 +1356,42 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
+      <c r="B15" s="22">
         <v>8</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="7">
         <v>207.96083333333334</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="7">
         <v>2495.5300000000002</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="13">
         <f t="shared" si="4"/>
         <v>2.9565491426347512E-2</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <v>225</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <f t="shared" si="0"/>
         <v>2699.9999999999995</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="9">
         <f t="shared" si="6"/>
         <v>1.0819344988840043</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="6">
         <f t="shared" si="1"/>
         <v>432.96083333333331</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="6">
         <f t="shared" si="5"/>
         <v>5195.53</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="13">
         <f t="shared" si="2"/>
         <v>6.8572501787058621E-2</v>
       </c>
@@ -1398,42 +1404,42 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="20">
+      <c r="B16" s="22">
         <v>16</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="7">
         <v>170.57666666666668</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="7">
         <v>2046.92</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="13">
         <f t="shared" si="4"/>
         <v>2.4250638425672801E-2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>-60</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <f t="shared" si="0"/>
         <v>-720</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="9">
         <f t="shared" si="6"/>
         <v>-0.35174799210521168</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="6">
         <f t="shared" si="1"/>
         <v>110.57666666666668</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="6">
         <f t="shared" si="5"/>
         <v>1326.92</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="13">
         <f t="shared" si="2"/>
         <v>1.7513174608034952E-2</v>
       </c>
@@ -1446,42 +1452,42 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="20">
+      <c r="B17" s="22">
         <v>49</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="7">
         <v>163.26583333333335</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="7">
         <v>1959.19</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="13">
         <f t="shared" si="4"/>
         <v>2.3211267805871207E-2</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <v>-25</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="3">
         <f t="shared" si="0"/>
         <v>-300</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="9">
         <f t="shared" si="6"/>
         <v>-0.15312450553545087</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="6">
         <f t="shared" si="1"/>
         <v>138.26583333333335</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="6">
         <f t="shared" si="5"/>
         <v>1659.19</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="13">
         <f t="shared" si="2"/>
         <v>2.1898595377193436E-2</v>
       </c>
@@ -1494,42 +1500,42 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="20">
+      <c r="B18" s="22">
         <v>48</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="7">
         <v>126.62833333333333</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="7">
         <v>1519.54</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="13">
         <f t="shared" si="4"/>
         <v>1.8002567327177831E-2</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <v>-30</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <f t="shared" si="0"/>
         <v>-360</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="9">
         <f t="shared" si="6"/>
         <v>-0.2369138028613923</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="6">
         <f t="shared" si="1"/>
         <v>96.62833333333333</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="6">
         <f t="shared" si="5"/>
         <v>1159.54</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="13">
         <f t="shared" si="2"/>
         <v>1.5304032258916021E-2</v>
       </c>
@@ -1539,37 +1545,40 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="20">
+      <c r="B19" s="22">
         <v>7</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="7">
         <v>88.006666666666661</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="7">
         <v>1056.08</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="13">
         <f t="shared" si="4"/>
         <v>1.2511780738174686E-2</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="7">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="6">
         <f t="shared" si="1"/>
         <v>88.006666666666661</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="6">
         <f t="shared" si="5"/>
         <v>1056.08</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="13">
         <f t="shared" si="2"/>
         <v>1.3938529406485357E-2</v>
       </c>
@@ -1579,42 +1588,42 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="20">
+      <c r="B20" s="22">
         <v>41</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="7">
         <v>48.75</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="7">
         <v>585</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="13">
         <f t="shared" si="4"/>
         <v>6.930717115968669E-3</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>15</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="9">
         <f t="shared" si="6"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="6">
         <f t="shared" si="1"/>
         <v>63.75</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="6">
         <f t="shared" si="5"/>
         <v>765</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="13">
         <f t="shared" si="2"/>
         <v>1.0096749295471271E-2</v>
       </c>
@@ -1624,42 +1633,42 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
+      <c r="B21" s="22">
         <v>54</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="7">
         <v>40.06</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="7">
         <v>480.72</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="13">
         <f t="shared" si="4"/>
         <v>5.6952723623734337E-3</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="3">
         <v>-25</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="3">
         <f t="shared" si="0"/>
         <v>-300</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="9">
         <f t="shared" si="6"/>
         <v>-0.62406390414378432</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="6">
         <f t="shared" si="1"/>
         <v>15.060000000000002</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="6">
         <f t="shared" si="5"/>
         <v>180.72000000000003</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="13">
         <f t="shared" si="2"/>
         <v>2.3852085394478017E-3</v>
       </c>
@@ -1672,42 +1681,42 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="20">
+      <c r="B22" s="22">
         <v>24</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="7">
         <v>32.738333333333337</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="7">
         <v>392.86</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="13">
         <f t="shared" si="4"/>
         <v>4.6543615832127377E-3</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <v>-15</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <f t="shared" si="0"/>
         <v>-179.99999999999997</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="9">
         <f t="shared" si="6"/>
         <v>-0.45817848597464739</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="6">
         <f t="shared" si="1"/>
         <v>17.738333333333337</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="6">
         <f t="shared" si="5"/>
         <v>212.86000000000004</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="13">
         <f t="shared" si="2"/>
         <v>2.8094039935085166E-3</v>
       </c>
@@ -1718,36 +1727,36 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="7">
         <v>0.01</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="7">
         <v>0.01</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="13">
         <f t="shared" si="4"/>
         <v>1.1847379685416529E-7</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>30</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <f t="shared" ref="H23" si="7">K23-E23</f>
         <v>360.11</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="4">
+      <c r="I23" s="9"/>
+      <c r="J23" s="6">
         <f t="shared" ref="J23" si="8">D23+G23</f>
         <v>30.01</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="6">
         <f t="shared" si="5"/>
         <v>360.12</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="13">
         <f t="shared" si="2"/>
         <v>4.752995236974005E-3</v>
       </c>
@@ -1759,48 +1768,48 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="11"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="13"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D26" s="4">
+      <c r="D26" s="6">
         <f>SUM(D3:D25)</f>
         <v>7033.9133333333339</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="6">
         <f>SUM(E3:E25)</f>
         <v>84406.849999999991</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="2">
+      <c r="F26" s="6"/>
+      <c r="G26" s="3">
         <f>SUM(G3:G24)</f>
         <v>-720</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <f t="shared" ref="H26" si="9">K26-E26</f>
         <v>-8639.8899999999849</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="9">
         <f t="shared" ref="I26" si="10">1-(J26/D26)</f>
         <v>0.10236122708364337</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="6">
         <f>SUM(J3:J25)</f>
         <v>6313.9133333333339</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="6">
         <f>SUM(K3:K25)</f>
         <v>75766.960000000006</v>
       </c>
@@ -1809,7 +1818,7 @@
       <c r="J29" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="6">
         <f>E26-K26</f>
         <v>8639.8899999999849</v>
       </c>
@@ -1818,7 +1827,7 @@
       <c r="J30" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="4">
         <v>-8050</v>
       </c>
     </row>
@@ -1826,7 +1835,7 @@
       <c r="J32" t="s">
         <v>26</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="8">
         <f>K29+K30</f>
         <v>589.88999999998487</v>
       </c>
@@ -1859,46 +1868,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="24" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2053,114 +2062,114 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="8">
+      <c r="B3" s="10">
         <v>4526.09</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="17">
         <v>27</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="19">
         <v>2325.0410999999999</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="19">
         <v>62776.11</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="B4" s="10">
         <v>22436.41</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="17">
         <v>1</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="19">
         <v>6340</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="19">
         <v>6340</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+      <c r="B5" s="10">
         <v>58465.37</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="17">
         <v>27</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="19">
         <v>191.9915</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="19">
         <v>5183.7700000000004</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="15">
+      <c r="D6" s="17">
         <v>12</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="19">
         <v>10.583299999999999</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="19">
         <v>127</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="15">
+      <c r="D7" s="17">
         <v>25</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="19">
         <v>9.0399999999999994E-2</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="19">
         <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
+      <c r="B9" s="10">
         <f>SUM(B3:B6)</f>
         <v>85427.87</v>
       </c>
       <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="20">
         <f>SUM(G3:G7)</f>
         <v>74429.14</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="10">
         <f>G9-B9</f>
         <v>-10998.729999999996</v>
       </c>

</xml_diff>